<commit_message>
moving to final touching
</commit_message>
<xml_diff>
--- a/1_Requirements/ProjectDistribution.xlsx
+++ b/1_Requirements/ProjectDistribution.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
   <si>
     <t>PROJECT NAME</t>
   </si>
@@ -34,6 +34,9 @@
     <t>April 08, 2021</t>
   </si>
   <si>
+    <t>April 16, 2021</t>
+  </si>
+  <si>
     <t>TASK ID</t>
   </si>
   <si>
@@ -74,9 +77,6 @@
   </si>
   <si>
     <t>April 16,2021</t>
-  </si>
-  <si>
-    <t>April 17,2021</t>
   </si>
   <si>
     <t>Creating Template</t>
@@ -112,16 +112,22 @@
     <t>April 13, 2021</t>
   </si>
   <si>
-    <t>TESTING</t>
-  </si>
-  <si>
-    <t>Final Testing</t>
-  </si>
-  <si>
-    <t>April 16, 2021</t>
-  </si>
-  <si>
-    <t>April 17, 2021</t>
+    <t>Working on github
+Like raising Issues</t>
+  </si>
+  <si>
+    <t>April 14, 2021</t>
+  </si>
+  <si>
+    <t>Working with math
+ quationaire</t>
+  </si>
+  <si>
+    <t>April 15, 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TESTING AND FINAL TOUCH
+</t>
   </si>
 </sst>
 </file>
@@ -129,10 +135,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -172,14 +178,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -187,60 +193,23 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -263,7 +232,22 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -293,6 +277,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
@@ -300,7 +292,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -341,79 +347,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -425,103 +509,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -546,41 +552,6 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -641,18 +612,59 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -661,143 +673,137 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -832,6 +838,12 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1153,10 +1165,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1175,10 +1187,9 @@
     <col min="12" max="12" width="6.14285714285714" customWidth="1"/>
     <col min="13" max="13" width="5.71428571428571" customWidth="1"/>
     <col min="14" max="14" width="5.85714285714286" customWidth="1"/>
-    <col min="15" max="15" width="4.85714285714286" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="54" customHeight="1" spans="2:15">
+    <row r="1" ht="54" customHeight="1" spans="2:14">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1200,17 +1211,20 @@
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
     </row>
-    <row r="2" ht="28" customHeight="1" spans="2:15">
+    <row r="2" ht="28" customHeight="1" spans="2:14">
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1"/>
+      <c r="C2" s="1">
+        <v>9</v>
+      </c>
       <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="1"/>
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
@@ -1220,9 +1234,8 @@
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
     </row>
-    <row r="3" spans="6:15">
+    <row r="3" spans="6:14">
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
@@ -1232,9 +1245,8 @@
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
     </row>
-    <row r="4" spans="6:15">
+    <row r="4" spans="6:14">
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -1244,56 +1256,52 @@
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
     </row>
-    <row r="5" ht="83" customHeight="1" spans="1:15">
+    <row r="5" ht="83" customHeight="1" spans="1:14">
       <c r="A5" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="O5" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:14">
       <c r="A6" s="6">
         <v>1</v>
       </c>
@@ -1318,9 +1326,8 @@
       <c r="L6" s="9"/>
       <c r="M6" s="9"/>
       <c r="N6" s="9"/>
-      <c r="O6" s="9"/>
     </row>
-    <row r="7" ht="75" spans="1:15">
+    <row r="7" ht="75" spans="1:14">
       <c r="A7" s="6">
         <v>2</v>
       </c>
@@ -1345,9 +1352,8 @@
       <c r="L7" s="9"/>
       <c r="M7" s="9"/>
       <c r="N7" s="9"/>
-      <c r="O7" s="9"/>
     </row>
-    <row r="8" ht="60" spans="1:15">
+    <row r="8" ht="60" spans="1:14">
       <c r="A8" s="6">
         <v>3</v>
       </c>
@@ -1372,9 +1378,8 @@
       <c r="L8" s="9"/>
       <c r="M8" s="9"/>
       <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
     </row>
-    <row r="9" ht="60" spans="1:15">
+    <row r="9" ht="60" spans="1:14">
       <c r="A9" s="6">
         <v>4</v>
       </c>
@@ -1399,9 +1404,8 @@
       <c r="L9" s="9"/>
       <c r="M9" s="9"/>
       <c r="N9" s="9"/>
-      <c r="O9" s="9"/>
     </row>
-    <row r="10" ht="18" customHeight="1" spans="1:15">
+    <row r="10" ht="18" customHeight="1" spans="1:14">
       <c r="A10" s="6">
         <v>5</v>
       </c>
@@ -1426,35 +1430,49 @@
       <c r="L10" s="9"/>
       <c r="M10" s="9"/>
       <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" ht="30" spans="1:14">
       <c r="A11" s="6">
         <v>6</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
+      <c r="B11" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="7">
+        <v>1</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>32</v>
+      </c>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
       <c r="J11" s="9"/>
       <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
+      <c r="L11" s="8"/>
       <c r="M11" s="9"/>
       <c r="N11" s="9"/>
-      <c r="O11" s="9"/>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" ht="30" spans="1:14">
       <c r="A12" s="6">
         <v>7</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
+      <c r="B12" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="7">
+        <v>1</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>34</v>
+      </c>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
@@ -1462,20 +1480,25 @@
       <c r="J12" s="9"/>
       <c r="K12" s="9"/>
       <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
+      <c r="M12" s="8"/>
       <c r="N12" s="9"/>
-      <c r="O12" s="9"/>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" ht="45" spans="1:14">
       <c r="A13" s="6">
         <v>8</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
+      <c r="B13" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="7">
+        <v>2</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>6</v>
+      </c>
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
@@ -1484,54 +1507,7 @@
       <c r="K13" s="9"/>
       <c r="L13" s="9"/>
       <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
-    </row>
-    <row r="14" spans="1:15">
-      <c r="A14" s="6">
-        <v>9</v>
-      </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="9"/>
-    </row>
-    <row r="15" spans="1:15">
-      <c r="A15" s="6">
-        <v>10</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="7">
-        <v>1</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="9"/>
-      <c r="M15" s="9"/>
-      <c r="N15" s="9"/>
-      <c r="O15" s="9"/>
+      <c r="N13" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>